<commit_message>
Aggiornato deliveryopenfiber.xlsx da lbianco via Streamlit
</commit_message>
<xml_diff>
--- a/deliveryopenfiber.xlsx
+++ b/deliveryopenfiber.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$AI$369</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$AI$500</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17465" uniqueCount="2536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18305" uniqueCount="2650">
   <si>
     <t>Codice</t>
   </si>
@@ -7625,6 +7625,348 @@
   </si>
   <si>
     <t>RUSSO GIOVANNI</t>
+  </si>
+  <si>
+    <t>DEL1003550358</t>
+  </si>
+  <si>
+    <t>4224696945530035971</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:56</t>
+  </si>
+  <si>
+    <t>ALESSIA VENERINI</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:30</t>
+  </si>
+  <si>
+    <t>18/08/2025 13:30</t>
+  </si>
+  <si>
+    <t>OPI_3721046</t>
+  </si>
+  <si>
+    <t>19_089_089017_8000970111_59/D</t>
+  </si>
+  <si>
+    <t>SR_01/VOD_0018</t>
+  </si>
+  <si>
+    <t>SR_01/02e22-SP_02</t>
+  </si>
+  <si>
+    <t>SR_01/02e22/I754_VIA ALESSANDRO SPECCHI_59/D_1</t>
+  </si>
+  <si>
+    <t>DEL1003553747</t>
+  </si>
+  <si>
+    <t>4224696945508718080</t>
+  </si>
+  <si>
+    <t>18/08/2025 15:28</t>
+  </si>
+  <si>
+    <t>CARMELA RIZZA</t>
+  </si>
+  <si>
+    <t>07/08/2025 13:16</t>
+  </si>
+  <si>
+    <t>WN_9002064152</t>
+  </si>
+  <si>
+    <t>19_089_089017_8000970113_65</t>
+  </si>
+  <si>
+    <t>SR_01/WIN_0148</t>
+  </si>
+  <si>
+    <t>SR_01/06e24-SP_09</t>
+  </si>
+  <si>
+    <t>SR_01/06e24/I754_VIA ALCIBIADE_65_1_C</t>
+  </si>
+  <si>
+    <t>DEL1003566105</t>
+  </si>
+  <si>
+    <t>4224696945535864601</t>
+  </si>
+  <si>
+    <t>18/08/2025 10:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tisera warnakulasuriya krishan</t>
+  </si>
+  <si>
+    <t>18/08/2025 14:30</t>
+  </si>
+  <si>
+    <t>18/08/2025 16:30</t>
+  </si>
+  <si>
+    <t>12/08/2025 11:56</t>
+  </si>
+  <si>
+    <t>OPI_AP_186471</t>
+  </si>
+  <si>
+    <t>19_089_089017_8000971062_46</t>
+  </si>
+  <si>
+    <t>SR_01/VOD_0011</t>
+  </si>
+  <si>
+    <t>SR_01/03w31-SP_02</t>
+  </si>
+  <si>
+    <t>SR_01/03w31/I754_VIA MONTEGRAPPA_62</t>
+  </si>
+  <si>
+    <t>DEL1003557353</t>
+  </si>
+  <si>
+    <t>4224696945526859474</t>
+  </si>
+  <si>
+    <t>18/08/2025 12:48</t>
+  </si>
+  <si>
+    <t>PATRIZIA CANNARELLA</t>
+  </si>
+  <si>
+    <t>18/08/2025 18:00</t>
+  </si>
+  <si>
+    <t>08/08/2025 16:26</t>
+  </si>
+  <si>
+    <t>PORTOPALO DI CAPO PASSERO</t>
+  </si>
+  <si>
+    <t>ENE_00000717487</t>
+  </si>
+  <si>
+    <t>SRBXA</t>
+  </si>
+  <si>
+    <t>19_089_089020_8000967678_61</t>
+  </si>
+  <si>
+    <t>SRBXA/EOF_0003</t>
+  </si>
+  <si>
+    <t>M257_CNO5-SP_01</t>
+  </si>
+  <si>
+    <t>M257_CNO5/M257_141</t>
+  </si>
+  <si>
+    <t>DEL1003579554</t>
+  </si>
+  <si>
+    <t>4224696945505308507</t>
+  </si>
+  <si>
+    <t>18/08/2025 14:28</t>
+  </si>
+  <si>
+    <t>NATALIYA PETRENKO</t>
+  </si>
+  <si>
+    <t>22/08/2025 11:30</t>
+  </si>
+  <si>
+    <t>22/08/2025 13:30</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:36</t>
+  </si>
+  <si>
+    <t>PACHINO</t>
+  </si>
+  <si>
+    <t>TLC_00000000173713</t>
+  </si>
+  <si>
+    <t>SRBWA</t>
+  </si>
+  <si>
+    <t>19_089_089014_8000915960_47</t>
+  </si>
+  <si>
+    <t>SRBWA/EOF_0002</t>
+  </si>
+  <si>
+    <t>G211_CNO2-SP_01</t>
+  </si>
+  <si>
+    <t>G211_CNO2/G211_105</t>
+  </si>
+  <si>
+    <t>DEL1003551917</t>
+  </si>
+  <si>
+    <t>4224696945530038467</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:48</t>
+  </si>
+  <si>
+    <t>ALESSIA FRIDA PERILLO</t>
+  </si>
+  <si>
+    <t>06/08/2025 21:06</t>
+  </si>
+  <si>
+    <t>WN_9002076917</t>
+  </si>
+  <si>
+    <t>19_089_089017_8000956037_6</t>
+  </si>
+  <si>
+    <t>SR_01/WIN_0135</t>
+  </si>
+  <si>
+    <t>SR_01/05e22-SP_06</t>
+  </si>
+  <si>
+    <t>SR_01/05e22/I754_RONCO I BOTTAI_9</t>
+  </si>
+  <si>
+    <t>DEL1003559711</t>
+  </si>
+  <si>
+    <t>4224696945532985061</t>
+  </si>
+  <si>
+    <t>18/08/2025 09:28</t>
+  </si>
+  <si>
+    <t>LUCIANO SACCO</t>
+  </si>
+  <si>
+    <t>18/08/2025 08:30</t>
+  </si>
+  <si>
+    <t>18/08/2025 10:30</t>
+  </si>
+  <si>
+    <t>09/08/2025 16:16</t>
+  </si>
+  <si>
+    <t>ENE_00000723415</t>
+  </si>
+  <si>
+    <t>19_089_089017_8000916291_8</t>
+  </si>
+  <si>
+    <t>SR_01/EOF_0083</t>
+  </si>
+  <si>
+    <t>SR_01/05w13-SP_08</t>
+  </si>
+  <si>
+    <t>SR_01/05w13/I754_VIA DELLA DOGANA_8_A_1</t>
+  </si>
+  <si>
+    <t>DEL1003562906</t>
+  </si>
+  <si>
+    <t>4224696945534949757</t>
+  </si>
+  <si>
+    <t>OSANI PONNAMPERUMAGE FERNANDO</t>
+  </si>
+  <si>
+    <t>9039295140825112</t>
+  </si>
+  <si>
+    <t>19_089_089017_8000916125_11</t>
+  </si>
+  <si>
+    <t>SR_01/SKY_0042</t>
+  </si>
+  <si>
+    <t>SR_01/05e24-SP_04</t>
+  </si>
+  <si>
+    <t>SR_01/05e24/I754_VIA MARIO GEMELLARO_5</t>
+  </si>
+  <si>
+    <t>DEL1003563013</t>
+  </si>
+  <si>
+    <t>4224696945534949793</t>
+  </si>
+  <si>
+    <t>18/08/2025 13:48</t>
+  </si>
+  <si>
+    <t>CONCETTA SALERNO</t>
+  </si>
+  <si>
+    <t>WN_9002080188</t>
+  </si>
+  <si>
+    <t>19_089_089017_8000970274_4</t>
+  </si>
+  <si>
+    <t>SR_01/WIN_0182</t>
+  </si>
+  <si>
+    <t>SR_01/03e34-SP_08</t>
+  </si>
+  <si>
+    <t>SR_01/03e34/I754_VIA ESCHILO_4_1</t>
+  </si>
+  <si>
+    <t>DEL1003554163</t>
+  </si>
+  <si>
+    <t>18/08/2025 16:18</t>
+  </si>
+  <si>
+    <t>DEL1003563391</t>
+  </si>
+  <si>
+    <t>4224696945534949945</t>
+  </si>
+  <si>
+    <t>18/08/2025 12:16</t>
+  </si>
+  <si>
+    <t>WN_9002080215</t>
+  </si>
+  <si>
+    <t>DEL1003568807</t>
+  </si>
+  <si>
+    <t>4224696945536624041</t>
+  </si>
+  <si>
+    <t>18/08/2025 09:48</t>
+  </si>
+  <si>
+    <t>GIUSEPPE RIO</t>
+  </si>
+  <si>
+    <t>13/08/2025 11:46</t>
+  </si>
+  <si>
+    <t>ENE_00000725570</t>
+  </si>
+  <si>
+    <t>19_089_089018_8000967613_8</t>
+  </si>
+  <si>
+    <t>SR_09/02e12-SP_01</t>
+  </si>
+  <si>
+    <t>SR_09/02e12/SR_09/01w12/I785_055</t>
   </si>
 </sst>
 </file>
@@ -7955,10 +8297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI500"/>
+  <dimension ref="A1:AI524"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A448" sqref="A448:AI500"/>
+    <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
+      <selection activeCell="D507" sqref="D507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -61365,12 +61707,2576 @@
         <v>57</v>
       </c>
     </row>
+    <row r="501" spans="1:35">
+      <c r="A501" s="1" t="s">
+        <v>2536</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D501" s="1" t="s">
+        <v>2538</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>1901</v>
+      </c>
+      <c r="F501" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G501" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H501" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="I501" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J501" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K501" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L501" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M501" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N501" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="O501" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="P501" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q501" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R501" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S501" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T501" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U501" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V501" s="1" t="s">
+        <v>2542</v>
+      </c>
+      <c r="W501" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="X501" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y501" s="1" t="s">
+        <v>2543</v>
+      </c>
+      <c r="Z501" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA501" s="1" t="s">
+        <v>2544</v>
+      </c>
+      <c r="AB501" s="1" t="s">
+        <v>2545</v>
+      </c>
+      <c r="AC501" s="1" t="s">
+        <v>2546</v>
+      </c>
+      <c r="AD501" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE501" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF501" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG501" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH501" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI501" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="502" spans="1:35">
+      <c r="A502" s="1" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>2548</v>
+      </c>
+      <c r="C502" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D502" s="1" t="s">
+        <v>2549</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>1901</v>
+      </c>
+      <c r="F502" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G502" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H502" s="1" t="s">
+        <v>2550</v>
+      </c>
+      <c r="I502" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J502" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K502" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L502" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M502" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N502" s="1" t="s">
+        <v>2551</v>
+      </c>
+      <c r="O502" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P502" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q502" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R502" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S502" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T502" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U502" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V502" s="1" t="s">
+        <v>2552</v>
+      </c>
+      <c r="W502" s="1" t="s">
+        <v>2548</v>
+      </c>
+      <c r="X502" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y502" s="1" t="s">
+        <v>2553</v>
+      </c>
+      <c r="Z502" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA502" s="1" t="s">
+        <v>2554</v>
+      </c>
+      <c r="AB502" s="1" t="s">
+        <v>2555</v>
+      </c>
+      <c r="AC502" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="AD502" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE502" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF502" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG502" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH502" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI502" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="503" spans="1:35">
+      <c r="A503" s="1" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D503" s="1" t="s">
+        <v>2559</v>
+      </c>
+      <c r="E503" s="1" t="s">
+        <v>1901</v>
+      </c>
+      <c r="F503" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G503" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H503" s="1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="I503" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J503" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="K503" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L503" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="M503" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N503" s="1" t="s">
+        <v>2563</v>
+      </c>
+      <c r="O503" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P503" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q503" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R503" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S503" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T503" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U503" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V503" s="1" t="s">
+        <v>2564</v>
+      </c>
+      <c r="W503" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="X503" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y503" s="1" t="s">
+        <v>2565</v>
+      </c>
+      <c r="Z503" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA503" s="1" t="s">
+        <v>2566</v>
+      </c>
+      <c r="AB503" s="1" t="s">
+        <v>2567</v>
+      </c>
+      <c r="AC503" s="1" t="s">
+        <v>2568</v>
+      </c>
+      <c r="AD503" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE503" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF503" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG503" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH503" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI503" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="504" spans="1:35">
+      <c r="A504" s="1" t="s">
+        <v>2569</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C504" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D504" s="1" t="s">
+        <v>2571</v>
+      </c>
+      <c r="E504" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F504" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G504" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H504" s="1" t="s">
+        <v>2572</v>
+      </c>
+      <c r="I504" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J504" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="K504" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L504" s="1" t="s">
+        <v>2573</v>
+      </c>
+      <c r="M504" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N504" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="O504" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P504" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q504" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R504" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S504" s="1" t="s">
+        <v>2575</v>
+      </c>
+      <c r="T504" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U504" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V504" s="1" t="s">
+        <v>2576</v>
+      </c>
+      <c r="W504" s="1" t="s">
+        <v>2570</v>
+      </c>
+      <c r="X504" s="1" t="s">
+        <v>2577</v>
+      </c>
+      <c r="Y504" s="1" t="s">
+        <v>2578</v>
+      </c>
+      <c r="Z504" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA504" s="1" t="s">
+        <v>2579</v>
+      </c>
+      <c r="AB504" s="1" t="s">
+        <v>2580</v>
+      </c>
+      <c r="AC504" s="1" t="s">
+        <v>2581</v>
+      </c>
+      <c r="AD504" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE504" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF504" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AG504" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH504" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AI504" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="505" spans="1:35">
+      <c r="A505" s="1" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>2583</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D505" s="1" t="s">
+        <v>2584</v>
+      </c>
+      <c r="E505" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F505" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G505" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H505" s="1" t="s">
+        <v>2585</v>
+      </c>
+      <c r="I505" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J505" s="1" t="s">
+        <v>2586</v>
+      </c>
+      <c r="K505" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L505" s="1" t="s">
+        <v>2587</v>
+      </c>
+      <c r="M505" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N505" s="1" t="s">
+        <v>2588</v>
+      </c>
+      <c r="O505" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P505" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q505" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R505" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S505" s="1" t="s">
+        <v>2589</v>
+      </c>
+      <c r="T505" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U505" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="V505" s="1" t="s">
+        <v>2590</v>
+      </c>
+      <c r="W505" s="1" t="s">
+        <v>2583</v>
+      </c>
+      <c r="X505" s="1" t="s">
+        <v>2591</v>
+      </c>
+      <c r="Y505" s="1" t="s">
+        <v>2592</v>
+      </c>
+      <c r="Z505" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA505" s="1" t="s">
+        <v>2593</v>
+      </c>
+      <c r="AB505" s="1" t="s">
+        <v>2594</v>
+      </c>
+      <c r="AC505" s="1" t="s">
+        <v>2595</v>
+      </c>
+      <c r="AD505" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE505" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF505" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AG505" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH505" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AI505" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="506" spans="1:35">
+      <c r="A506" s="1" t="s">
+        <v>2596</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C506" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D506" s="1" t="s">
+        <v>2598</v>
+      </c>
+      <c r="E506" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F506" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G506" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H506" s="1" t="s">
+        <v>2599</v>
+      </c>
+      <c r="I506" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J506" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K506" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L506" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M506" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N506" s="1" t="s">
+        <v>2600</v>
+      </c>
+      <c r="O506" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P506" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q506" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R506" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S506" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T506" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U506" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V506" s="1" t="s">
+        <v>2601</v>
+      </c>
+      <c r="W506" s="1" t="s">
+        <v>2597</v>
+      </c>
+      <c r="X506" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y506" s="1" t="s">
+        <v>2602</v>
+      </c>
+      <c r="Z506" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA506" s="1" t="s">
+        <v>2603</v>
+      </c>
+      <c r="AB506" s="1" t="s">
+        <v>2604</v>
+      </c>
+      <c r="AC506" s="1" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AD506" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE506" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF506" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG506" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH506" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI506" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="507" spans="1:35">
+      <c r="A507" s="1" t="s">
+        <v>2606</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C507" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D507" s="1" t="s">
+        <v>2608</v>
+      </c>
+      <c r="E507" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F507" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G507" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H507" s="1" t="s">
+        <v>2609</v>
+      </c>
+      <c r="I507" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J507" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K507" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L507" s="1" t="s">
+        <v>2611</v>
+      </c>
+      <c r="M507" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N507" s="1" t="s">
+        <v>2612</v>
+      </c>
+      <c r="O507" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P507" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q507" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R507" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S507" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T507" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U507" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V507" s="1" t="s">
+        <v>2613</v>
+      </c>
+      <c r="W507" s="1" t="s">
+        <v>2607</v>
+      </c>
+      <c r="X507" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y507" s="1" t="s">
+        <v>2614</v>
+      </c>
+      <c r="Z507" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA507" s="1" t="s">
+        <v>2615</v>
+      </c>
+      <c r="AB507" s="1" t="s">
+        <v>2616</v>
+      </c>
+      <c r="AC507" s="1" t="s">
+        <v>2617</v>
+      </c>
+      <c r="AD507" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE507" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF507" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG507" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH507" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI507" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="508" spans="1:35">
+      <c r="A508" s="1" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>2619</v>
+      </c>
+      <c r="C508" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D508" s="1" t="s">
+        <v>2559</v>
+      </c>
+      <c r="E508" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F508" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G508" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H508" s="1" t="s">
+        <v>2620</v>
+      </c>
+      <c r="I508" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J508" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K508" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L508" s="1" t="s">
+        <v>2611</v>
+      </c>
+      <c r="M508" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N508" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="O508" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P508" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q508" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R508" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S508" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T508" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U508" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V508" s="1" t="s">
+        <v>2621</v>
+      </c>
+      <c r="W508" s="1" t="s">
+        <v>2619</v>
+      </c>
+      <c r="X508" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y508" s="1" t="s">
+        <v>2622</v>
+      </c>
+      <c r="Z508" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA508" s="1" t="s">
+        <v>2623</v>
+      </c>
+      <c r="AB508" s="1" t="s">
+        <v>2624</v>
+      </c>
+      <c r="AC508" s="1" t="s">
+        <v>2625</v>
+      </c>
+      <c r="AD508" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE508" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF508" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG508" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH508" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI508" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="509" spans="1:35">
+      <c r="A509" s="1" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>2627</v>
+      </c>
+      <c r="C509" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D509" s="1" t="s">
+        <v>2628</v>
+      </c>
+      <c r="E509" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F509" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G509" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H509" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="I509" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J509" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K509" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L509" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M509" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N509" s="1" t="s">
+        <v>2144</v>
+      </c>
+      <c r="O509" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P509" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q509" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R509" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S509" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T509" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U509" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V509" s="1" t="s">
+        <v>2630</v>
+      </c>
+      <c r="W509" s="1" t="s">
+        <v>2627</v>
+      </c>
+      <c r="X509" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y509" s="1" t="s">
+        <v>2631</v>
+      </c>
+      <c r="Z509" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA509" s="1" t="s">
+        <v>2632</v>
+      </c>
+      <c r="AB509" s="1" t="s">
+        <v>2633</v>
+      </c>
+      <c r="AC509" s="1" t="s">
+        <v>2634</v>
+      </c>
+      <c r="AD509" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE509" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF509" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG509" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH509" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI509" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="510" spans="1:35">
+      <c r="A510" s="1" t="s">
+        <v>2635</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C510" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D510" s="1" t="s">
+        <v>2636</v>
+      </c>
+      <c r="E510" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F510" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G510" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H510" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I510" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J510" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="K510" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L510" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="M510" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N510" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="O510" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P510" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q510" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R510" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S510" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="T510" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U510" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V510" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="W510" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="X510" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y510" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="Z510" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA510" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB510" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="AC510" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD510" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE510" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF510" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG510" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH510" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI510" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="511" spans="1:35">
+      <c r="A511" s="1" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C511" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D511" s="1" t="s">
+        <v>2639</v>
+      </c>
+      <c r="E511" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F511" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G511" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H511" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I511" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J511" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K511" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L511" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M511" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N511" s="1" t="s">
+        <v>2329</v>
+      </c>
+      <c r="O511" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P511" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q511" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R511" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S511" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T511" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U511" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V511" s="1" t="s">
+        <v>2640</v>
+      </c>
+      <c r="W511" s="1" t="s">
+        <v>2638</v>
+      </c>
+      <c r="X511" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y511" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z511" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA511" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB511" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC511" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD511" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE511" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF511" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG511" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH511" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI511" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="512" spans="1:35">
+      <c r="A512" s="1" t="s">
+        <v>2641</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>2642</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D512" s="1" t="s">
+        <v>2643</v>
+      </c>
+      <c r="E512" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F512" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G512" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H512" s="1" t="s">
+        <v>2644</v>
+      </c>
+      <c r="I512" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J512" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K512" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L512" s="1" t="s">
+        <v>2611</v>
+      </c>
+      <c r="M512" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N512" s="1" t="s">
+        <v>2645</v>
+      </c>
+      <c r="O512" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P512" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q512" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R512" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S512" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="T512" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U512" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V512" s="1" t="s">
+        <v>2646</v>
+      </c>
+      <c r="W512" s="1" t="s">
+        <v>2642</v>
+      </c>
+      <c r="X512" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y512" s="1" t="s">
+        <v>2647</v>
+      </c>
+      <c r="Z512" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA512" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="AB512" s="1" t="s">
+        <v>2648</v>
+      </c>
+      <c r="AC512" s="1" t="s">
+        <v>2649</v>
+      </c>
+      <c r="AD512" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE512" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF512" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG512" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH512" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI512" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="513" spans="1:35">
+      <c r="A513" s="1" t="s">
+        <v>2536</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C513" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D513" s="1" t="s">
+        <v>2538</v>
+      </c>
+      <c r="E513" s="1" t="s">
+        <v>1900</v>
+      </c>
+      <c r="F513" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G513" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H513" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="I513" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J513" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K513" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L513" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M513" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N513" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="O513" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="P513" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q513" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R513" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S513" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T513" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U513" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V513" s="1" t="s">
+        <v>2542</v>
+      </c>
+      <c r="W513" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="X513" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y513" s="1" t="s">
+        <v>2543</v>
+      </c>
+      <c r="Z513" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA513" s="1" t="s">
+        <v>2544</v>
+      </c>
+      <c r="AB513" s="1" t="s">
+        <v>2545</v>
+      </c>
+      <c r="AC513" s="1" t="s">
+        <v>2546</v>
+      </c>
+      <c r="AD513" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE513" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF513" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG513" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH513" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI513" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="514" spans="1:35">
+      <c r="A514" s="1" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>2548</v>
+      </c>
+      <c r="C514" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D514" s="1" t="s">
+        <v>2549</v>
+      </c>
+      <c r="E514" s="1" t="s">
+        <v>1900</v>
+      </c>
+      <c r="F514" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G514" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H514" s="1" t="s">
+        <v>2550</v>
+      </c>
+      <c r="I514" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J514" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K514" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L514" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M514" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N514" s="1" t="s">
+        <v>2551</v>
+      </c>
+      <c r="O514" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P514" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q514" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R514" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S514" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T514" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U514" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V514" s="1" t="s">
+        <v>2552</v>
+      </c>
+      <c r="W514" s="1" t="s">
+        <v>2548</v>
+      </c>
+      <c r="X514" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y514" s="1" t="s">
+        <v>2553</v>
+      </c>
+      <c r="Z514" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA514" s="1" t="s">
+        <v>2554</v>
+      </c>
+      <c r="AB514" s="1" t="s">
+        <v>2555</v>
+      </c>
+      <c r="AC514" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="AD514" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE514" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF514" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG514" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH514" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI514" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="515" spans="1:35">
+      <c r="A515" s="1" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C515" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D515" s="1" t="s">
+        <v>2559</v>
+      </c>
+      <c r="E515" s="1" t="s">
+        <v>1900</v>
+      </c>
+      <c r="F515" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G515" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H515" s="1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="I515" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J515" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="K515" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L515" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="M515" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N515" s="1" t="s">
+        <v>2563</v>
+      </c>
+      <c r="O515" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P515" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q515" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R515" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S515" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T515" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U515" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V515" s="1" t="s">
+        <v>2564</v>
+      </c>
+      <c r="W515" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="X515" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y515" s="1" t="s">
+        <v>2565</v>
+      </c>
+      <c r="Z515" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA515" s="1" t="s">
+        <v>2566</v>
+      </c>
+      <c r="AB515" s="1" t="s">
+        <v>2567</v>
+      </c>
+      <c r="AC515" s="1" t="s">
+        <v>2568</v>
+      </c>
+      <c r="AD515" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE515" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF515" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG515" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH515" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI515" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="516" spans="1:35">
+      <c r="A516" s="1" t="s">
+        <v>2569</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C516" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D516" s="1" t="s">
+        <v>2571</v>
+      </c>
+      <c r="E516" s="1" t="s">
+        <v>1907</v>
+      </c>
+      <c r="F516" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G516" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H516" s="1" t="s">
+        <v>2572</v>
+      </c>
+      <c r="I516" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J516" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="K516" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L516" s="1" t="s">
+        <v>2573</v>
+      </c>
+      <c r="M516" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N516" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="O516" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P516" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q516" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R516" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S516" s="1" t="s">
+        <v>2575</v>
+      </c>
+      <c r="T516" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U516" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V516" s="1" t="s">
+        <v>2576</v>
+      </c>
+      <c r="W516" s="1" t="s">
+        <v>2570</v>
+      </c>
+      <c r="X516" s="1" t="s">
+        <v>2577</v>
+      </c>
+      <c r="Y516" s="1" t="s">
+        <v>2578</v>
+      </c>
+      <c r="Z516" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA516" s="1" t="s">
+        <v>2579</v>
+      </c>
+      <c r="AB516" s="1" t="s">
+        <v>2580</v>
+      </c>
+      <c r="AC516" s="1" t="s">
+        <v>2581</v>
+      </c>
+      <c r="AD516" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE516" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF516" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AG516" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH516" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AI516" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="517" spans="1:35">
+      <c r="A517" s="1" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>2583</v>
+      </c>
+      <c r="C517" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D517" s="1" t="s">
+        <v>2584</v>
+      </c>
+      <c r="E517" s="1" t="s">
+        <v>1907</v>
+      </c>
+      <c r="F517" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G517" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H517" s="1" t="s">
+        <v>2585</v>
+      </c>
+      <c r="I517" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J517" s="1" t="s">
+        <v>2586</v>
+      </c>
+      <c r="K517" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L517" s="1" t="s">
+        <v>2587</v>
+      </c>
+      <c r="M517" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N517" s="1" t="s">
+        <v>2588</v>
+      </c>
+      <c r="O517" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P517" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q517" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R517" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S517" s="1" t="s">
+        <v>2589</v>
+      </c>
+      <c r="T517" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U517" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="V517" s="1" t="s">
+        <v>2590</v>
+      </c>
+      <c r="W517" s="1" t="s">
+        <v>2583</v>
+      </c>
+      <c r="X517" s="1" t="s">
+        <v>2591</v>
+      </c>
+      <c r="Y517" s="1" t="s">
+        <v>2592</v>
+      </c>
+      <c r="Z517" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA517" s="1" t="s">
+        <v>2593</v>
+      </c>
+      <c r="AB517" s="1" t="s">
+        <v>2594</v>
+      </c>
+      <c r="AC517" s="1" t="s">
+        <v>2595</v>
+      </c>
+      <c r="AD517" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE517" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF517" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AG517" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH517" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AI517" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="518" spans="1:35">
+      <c r="A518" s="1" t="s">
+        <v>2596</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C518" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D518" s="1" t="s">
+        <v>2598</v>
+      </c>
+      <c r="E518" s="1" t="s">
+        <v>1903</v>
+      </c>
+      <c r="F518" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G518" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H518" s="1" t="s">
+        <v>2599</v>
+      </c>
+      <c r="I518" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J518" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K518" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L518" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M518" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N518" s="1" t="s">
+        <v>2600</v>
+      </c>
+      <c r="O518" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P518" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q518" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R518" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S518" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T518" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U518" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V518" s="1" t="s">
+        <v>2601</v>
+      </c>
+      <c r="W518" s="1" t="s">
+        <v>2597</v>
+      </c>
+      <c r="X518" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y518" s="1" t="s">
+        <v>2602</v>
+      </c>
+      <c r="Z518" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA518" s="1" t="s">
+        <v>2603</v>
+      </c>
+      <c r="AB518" s="1" t="s">
+        <v>2604</v>
+      </c>
+      <c r="AC518" s="1" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AD518" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE518" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF518" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG518" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH518" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI518" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="519" spans="1:35">
+      <c r="A519" s="1" t="s">
+        <v>2606</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C519" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D519" s="1" t="s">
+        <v>2608</v>
+      </c>
+      <c r="E519" s="1" t="s">
+        <v>1903</v>
+      </c>
+      <c r="F519" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G519" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H519" s="1" t="s">
+        <v>2609</v>
+      </c>
+      <c r="I519" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J519" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K519" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L519" s="1" t="s">
+        <v>2611</v>
+      </c>
+      <c r="M519" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N519" s="1" t="s">
+        <v>2612</v>
+      </c>
+      <c r="O519" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P519" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q519" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R519" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S519" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T519" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U519" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V519" s="1" t="s">
+        <v>2613</v>
+      </c>
+      <c r="W519" s="1" t="s">
+        <v>2607</v>
+      </c>
+      <c r="X519" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y519" s="1" t="s">
+        <v>2614</v>
+      </c>
+      <c r="Z519" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA519" s="1" t="s">
+        <v>2615</v>
+      </c>
+      <c r="AB519" s="1" t="s">
+        <v>2616</v>
+      </c>
+      <c r="AC519" s="1" t="s">
+        <v>2617</v>
+      </c>
+      <c r="AD519" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE519" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF519" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG519" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH519" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI519" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="520" spans="1:35">
+      <c r="A520" s="1" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>2619</v>
+      </c>
+      <c r="C520" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D520" s="1" t="s">
+        <v>2559</v>
+      </c>
+      <c r="E520" s="1" t="s">
+        <v>1903</v>
+      </c>
+      <c r="F520" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G520" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H520" s="1" t="s">
+        <v>2620</v>
+      </c>
+      <c r="I520" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J520" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K520" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L520" s="1" t="s">
+        <v>2611</v>
+      </c>
+      <c r="M520" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N520" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="O520" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P520" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q520" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R520" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S520" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T520" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U520" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V520" s="1" t="s">
+        <v>2621</v>
+      </c>
+      <c r="W520" s="1" t="s">
+        <v>2619</v>
+      </c>
+      <c r="X520" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y520" s="1" t="s">
+        <v>2622</v>
+      </c>
+      <c r="Z520" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA520" s="1" t="s">
+        <v>2623</v>
+      </c>
+      <c r="AB520" s="1" t="s">
+        <v>2624</v>
+      </c>
+      <c r="AC520" s="1" t="s">
+        <v>2625</v>
+      </c>
+      <c r="AD520" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE520" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF520" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG520" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH520" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI520" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="521" spans="1:35">
+      <c r="A521" s="1" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>2627</v>
+      </c>
+      <c r="C521" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D521" s="1" t="s">
+        <v>2628</v>
+      </c>
+      <c r="E521" s="1" t="s">
+        <v>1903</v>
+      </c>
+      <c r="F521" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G521" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H521" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="I521" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J521" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K521" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L521" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M521" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N521" s="1" t="s">
+        <v>2144</v>
+      </c>
+      <c r="O521" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P521" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q521" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R521" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S521" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T521" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U521" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V521" s="1" t="s">
+        <v>2630</v>
+      </c>
+      <c r="W521" s="1" t="s">
+        <v>2627</v>
+      </c>
+      <c r="X521" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y521" s="1" t="s">
+        <v>2631</v>
+      </c>
+      <c r="Z521" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA521" s="1" t="s">
+        <v>2632</v>
+      </c>
+      <c r="AB521" s="1" t="s">
+        <v>2633</v>
+      </c>
+      <c r="AC521" s="1" t="s">
+        <v>2634</v>
+      </c>
+      <c r="AD521" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE521" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF521" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG521" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH521" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI521" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="522" spans="1:35">
+      <c r="A522" s="1" t="s">
+        <v>2635</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C522" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D522" s="1" t="s">
+        <v>2636</v>
+      </c>
+      <c r="E522" s="1" t="s">
+        <v>1902</v>
+      </c>
+      <c r="F522" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G522" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H522" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I522" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J522" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="K522" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L522" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="M522" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N522" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="O522" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P522" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q522" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R522" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S522" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="T522" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U522" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V522" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="W522" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="X522" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y522" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="Z522" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA522" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB522" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="AC522" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD522" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE522" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF522" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG522" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH522" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI522" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="523" spans="1:35">
+      <c r="A523" s="1" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C523" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D523" s="1" t="s">
+        <v>2639</v>
+      </c>
+      <c r="E523" s="1" t="s">
+        <v>1902</v>
+      </c>
+      <c r="F523" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G523" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H523" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I523" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J523" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="K523" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L523" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="M523" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N523" s="1" t="s">
+        <v>2329</v>
+      </c>
+      <c r="O523" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P523" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q523" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R523" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S523" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T523" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U523" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V523" s="1" t="s">
+        <v>2640</v>
+      </c>
+      <c r="W523" s="1" t="s">
+        <v>2638</v>
+      </c>
+      <c r="X523" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y523" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z523" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA523" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB523" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC523" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD523" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE523" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF523" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG523" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH523" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI523" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="524" spans="1:35">
+      <c r="A524" s="1" t="s">
+        <v>2641</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>2642</v>
+      </c>
+      <c r="C524" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D524" s="1" t="s">
+        <v>2643</v>
+      </c>
+      <c r="E524" s="1" t="s">
+        <v>1902</v>
+      </c>
+      <c r="F524" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G524" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H524" s="1" t="s">
+        <v>2644</v>
+      </c>
+      <c r="I524" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J524" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K524" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L524" s="1" t="s">
+        <v>2611</v>
+      </c>
+      <c r="M524" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N524" s="1" t="s">
+        <v>2645</v>
+      </c>
+      <c r="O524" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P524" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q524" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R524" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S524" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="T524" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U524" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V524" s="1" t="s">
+        <v>2646</v>
+      </c>
+      <c r="W524" s="1" t="s">
+        <v>2642</v>
+      </c>
+      <c r="X524" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y524" s="1" t="s">
+        <v>2647</v>
+      </c>
+      <c r="Z524" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA524" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="AB524" s="1" t="s">
+        <v>2648</v>
+      </c>
+      <c r="AC524" s="1" t="s">
+        <v>2649</v>
+      </c>
+      <c r="AD524" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE524" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF524" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG524" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH524" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI524" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AI369">
-    <sortState ref="A2:AI369">
-      <sortCondition ref="D1:D369"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:AI500"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>